<commit_message>
Updated Glossary with regex helpers.
</commit_message>
<xml_diff>
--- a/Glossary Templates/Glossary_template_JP.xlsx
+++ b/Glossary Templates/Glossary_template_JP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Corbin\Documents\GitHub\AutoDeep\Glossary Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88777608-9639-4622-8754-7181BD918676}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A27B7ED-2FB2-47A7-A9C0-FAAE928066AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6415A24E-0804-47EC-BBE3-2CFC68F5F783}"/>
   </bookViews>
@@ -34,23 +34,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>…</t>
   </si>
   <si>
-    <t>#...</t>
-  </si>
-  <si>
     <t>……。</t>
   </si>
   <si>
     <t>──</t>
   </si>
   <si>
-    <t>#─</t>
-  </si>
-  <si>
     <t>。</t>
   </si>
   <si>
@@ -63,15 +57,9 @@
     <t>〝</t>
   </si>
   <si>
-    <t>#“</t>
-  </si>
-  <si>
     <t>〟</t>
   </si>
   <si>
-    <t>#”</t>
-  </si>
-  <si>
     <t>「</t>
   </si>
   <si>
@@ -81,109 +69,55 @@
     <t>《</t>
   </si>
   <si>
-    <t>#&lt;&lt;</t>
-  </si>
-  <si>
     <t>》</t>
   </si>
   <si>
-    <t>#&gt;&gt;</t>
-  </si>
-  <si>
     <t>『</t>
   </si>
   <si>
-    <t>#‘</t>
-  </si>
-  <si>
     <t>』</t>
   </si>
   <si>
-    <t>#’</t>
-  </si>
-  <si>
     <t>＊</t>
   </si>
   <si>
-    <t>#*</t>
-  </si>
-  <si>
     <t>●</t>
   </si>
   <si>
-    <t>#***</t>
-  </si>
-  <si>
     <t>？</t>
   </si>
   <si>
-    <t>#?</t>
-  </si>
-  <si>
     <t>！</t>
   </si>
   <si>
-    <t>#!</t>
-  </si>
-  <si>
     <t>０</t>
   </si>
   <si>
-    <t>#0</t>
-  </si>
-  <si>
     <t>１</t>
   </si>
   <si>
-    <t>#1</t>
-  </si>
-  <si>
     <t>２</t>
   </si>
   <si>
-    <t>#2</t>
-  </si>
-  <si>
     <t>３</t>
   </si>
   <si>
-    <t>#3</t>
-  </si>
-  <si>
     <t>４</t>
   </si>
   <si>
-    <t>#4</t>
-  </si>
-  <si>
     <t>５</t>
   </si>
   <si>
-    <t>#5</t>
-  </si>
-  <si>
     <t>６</t>
   </si>
   <si>
-    <t>#6</t>
-  </si>
-  <si>
     <t>７</t>
   </si>
   <si>
-    <t>#7</t>
-  </si>
-  <si>
     <t>８</t>
   </si>
   <si>
-    <t>#8</t>
-  </si>
-  <si>
     <t>９</t>
-  </si>
-  <si>
-    <t>#9</t>
   </si>
   <si>
     <t>Comment</t>
@@ -199,13 +133,133 @@
 If you wish for a certain replacement to be applied after all others, you can place it into a second group by using a ~ instead of a # .</t>
   </si>
   <si>
-    <t xml:space="preserve">~, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">~ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">~. </t>
+    <t>| terms do not get a space appended.</t>
+  </si>
+  <si>
+    <t>|...</t>
+  </si>
+  <si>
+    <t>|─</t>
+  </si>
+  <si>
+    <t>#.</t>
+  </si>
+  <si>
+    <t>#,</t>
+  </si>
+  <si>
+    <t>/| /</t>
+  </si>
+  <si>
+    <t>| “</t>
+  </si>
+  <si>
+    <t>/|” /</t>
+  </si>
+  <si>
+    <t>|&lt;&lt;</t>
+  </si>
+  <si>
+    <t>|&gt;&gt;</t>
+  </si>
+  <si>
+    <t>| ‘</t>
+  </si>
+  <si>
+    <t>/|’ /</t>
+  </si>
+  <si>
+    <t>|*</t>
+  </si>
+  <si>
+    <t>Replace Japanese space</t>
+  </si>
+  <si>
+    <t>/　/</t>
+  </si>
+  <si>
+    <t>Remove leading spaces</t>
+  </si>
+  <si>
+    <t>/^ /</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>Remove spaces before closing punctuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ([.,—’”])</t>
+  </si>
+  <si>
+    <t>:\1</t>
+  </si>
+  <si>
+    <t>Remove double spaces</t>
+  </si>
+  <si>
+    <t>/ +/</t>
+  </si>
+  <si>
+    <t>/: /</t>
+  </si>
+  <si>
+    <t>Remove trailing spaces</t>
+  </si>
+  <si>
+    <t>/ +$/</t>
+  </si>
+  <si>
+    <t>Get rid of multi-elipses when not at the beginning, to avoid breaking time passage markers.</t>
+  </si>
+  <si>
+    <t>([^.])\.{4,}</t>
+  </si>
+  <si>
+    <t>:\1…</t>
+  </si>
+  <si>
+    <t>|***</t>
+  </si>
+  <si>
+    <t>|?</t>
+  </si>
+  <si>
+    <t>|!</t>
+  </si>
+  <si>
+    <t>Convert fullwidth numbers</t>
+  </si>
+  <si>
+    <t>|0</t>
+  </si>
+  <si>
+    <t>|1</t>
+  </si>
+  <si>
+    <t>|2</t>
+  </si>
+  <si>
+    <t>|3</t>
+  </si>
+  <si>
+    <t>|4</t>
+  </si>
+  <si>
+    <t>|5</t>
+  </si>
+  <si>
+    <t>|6</t>
+  </si>
+  <si>
+    <t>|7</t>
+  </si>
+  <si>
+    <t>|8</t>
+  </si>
+  <si>
+    <t>|9</t>
   </si>
 </sst>
 </file>
@@ -605,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B646A47-EBB4-40AE-BD3D-6A1CF5AEE64C}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,7 +674,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="37.5" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -631,32 +685,34 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="25.5">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="2"/>
@@ -666,10 +722,10 @@
     <row r="4" spans="1:7">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="2"/>
@@ -679,10 +735,10 @@
     <row r="5" spans="1:7">
       <c r="A5" s="2"/>
       <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="2"/>
@@ -692,10 +748,10 @@
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="2"/>
@@ -705,10 +761,10 @@
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="2"/>
@@ -718,10 +774,10 @@
     <row r="8" spans="1:7">
       <c r="A8" s="2"/>
       <c r="B8" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="2"/>
@@ -731,10 +787,10 @@
     <row r="9" spans="1:7">
       <c r="A9" s="2"/>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="2"/>
@@ -744,10 +800,10 @@
     <row r="10" spans="1:7">
       <c r="A10" s="2"/>
       <c r="B10" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="2"/>
@@ -757,10 +813,10 @@
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
       <c r="B11" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="2"/>
@@ -770,10 +826,10 @@
     <row r="12" spans="1:7">
       <c r="A12" s="2"/>
       <c r="B12" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="2"/>
@@ -783,10 +839,10 @@
     <row r="13" spans="1:7">
       <c r="A13" s="2"/>
       <c r="B13" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="2"/>
@@ -796,10 +852,10 @@
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="2"/>
@@ -809,10 +865,10 @@
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
       <c r="B15" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="2"/>
@@ -822,10 +878,10 @@
     <row r="16" spans="1:7">
       <c r="A16" s="7"/>
       <c r="B16" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="7"/>
@@ -835,10 +891,10 @@
     <row r="17" spans="1:7">
       <c r="A17" s="7"/>
       <c r="B17" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="7"/>
@@ -846,12 +902,14 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="7"/>
+      <c r="A18" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="7"/>
@@ -859,12 +917,14 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="7"/>
+      <c r="A19" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="B19" s="5" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="7"/>
@@ -872,12 +932,14 @@
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="7"/>
-      <c r="B20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>29</v>
+      <c r="A20" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="7"/>
@@ -885,12 +947,14 @@
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="8"/>
-      <c r="B21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>31</v>
+      <c r="A21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
@@ -898,12 +962,14 @@
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="8"/>
-      <c r="B22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>33</v>
+      <c r="A22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="8"/>
@@ -911,12 +977,14 @@
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="8"/>
-      <c r="B23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>35</v>
+      <c r="A23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -924,12 +992,12 @@
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="8"/>
-      <c r="B24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>37</v>
+      <c r="A24" s="7"/>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
@@ -937,12 +1005,12 @@
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="8"/>
-      <c r="B25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>39</v>
+      <c r="A25" s="7"/>
+      <c r="B25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -950,12 +1018,12 @@
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="8"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="8"/>
@@ -963,12 +1031,14 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="8"/>
+      <c r="A27" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="B27" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
@@ -978,10 +1048,10 @@
     <row r="28" spans="1:7">
       <c r="A28" s="8"/>
       <c r="B28" s="3" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
@@ -991,10 +1061,10 @@
     <row r="29" spans="1:7">
       <c r="A29" s="8"/>
       <c r="B29" s="3" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
@@ -1004,10 +1074,10 @@
     <row r="30" spans="1:7">
       <c r="A30" s="8"/>
       <c r="B30" s="3" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="8"/>
@@ -1016,10 +1086,82 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="8"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="8"/>
       <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="8"/>
+      <c r="B32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="8"/>
+      <c r="B33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="8"/>
+      <c r="B34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="8"/>
+      <c r="B35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="8"/>
+      <c r="B36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="8"/>
+      <c r="B37" s="3"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>